<commit_message>
Add documentation examples to the repo
</commit_message>
<xml_diff>
--- a/evaluation/completeness/CompetencyQuestion_Completeness.xlsx
+++ b/evaluation/completeness/CompetencyQuestion_Completeness.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\ontologie-iot-urbani\evaluation\completeness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A732EA42-9CFC-4B95-98E0-B3A2E72D5953}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7427D7A1-5F1B-48A8-8868-4F34992942A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Competency Question" sheetId="2" r:id="rId1"/>
@@ -1170,15 +1170,6 @@
   </si>
   <si>
     <t>uiots:SharingMobilityTrip
-uiots:hasTripStartingPoint
-geo:lat/geo:long
-schema:startDate
-uiots:hasTripPoint
-uiots:tripRoute
-uiots:TripRoute</t>
-  </si>
-  <si>
-    <t>uiots:SharingMobilityTrip
 schema:startDate
 uiot:tripPerformedBy
 uiot:ServicePrivateUser
@@ -1661,6 +1652,15 @@
   </si>
   <si>
     <t>Cq-87</t>
+  </si>
+  <si>
+    <t>uiots:SharingMobilityTrip
+uiots:hasTripStartingPoint
+geo:lat/geo:long
+schema:startDate
+uiots:hasTripPoint
+uiots:hasTripRoute
+uiots:TripRoute</t>
   </si>
 </sst>
 </file>
@@ -2063,24 +2063,24 @@
   </sheetPr>
   <dimension ref="A1:T251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B29" sqref="B29"/>
+      <selection pane="topRight" activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="32" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="35.5546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="32" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="14.42578125" style="2"/>
+    <col min="7" max="7" width="23.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="14.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -2112,7 +2112,7 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="66" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="66" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -2160,10 +2160,10 @@
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="89.25" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2177,10 +2177,10 @@
         <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="63.75" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="66" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -2201,7 +2201,7 @@
       </c>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -2215,10 +2215,10 @@
         <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -2232,10 +2232,10 @@
         <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -2249,10 +2249,10 @@
         <v>23</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -2266,11 +2266,11 @@
         <v>110</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:20" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="66" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -2284,10 +2284,10 @@
         <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="89.25" x14ac:dyDescent="0.2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -2438,10 +2438,10 @@
         <v>168</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -2455,10 +2455,10 @@
         <v>29</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>34</v>
       </c>
@@ -2472,10 +2472,10 @@
         <v>30</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>35</v>
       </c>
@@ -2489,10 +2489,10 @@
         <v>31</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>36</v>
       </c>
@@ -2506,10 +2506,10 @@
         <v>32</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>37</v>
       </c>
@@ -2523,11 +2523,11 @@
         <v>32</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>39</v>
       </c>
@@ -2558,10 +2558,10 @@
         <v>195</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>40</v>
       </c>
@@ -2575,10 +2575,10 @@
         <v>195</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>41</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="7" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="7" customFormat="1" ht="79.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
         <v>46</v>
       </c>
@@ -2643,10 +2643,10 @@
         <v>66</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>47</v>
       </c>
@@ -2660,10 +2660,10 @@
         <v>48</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>49</v>
       </c>
@@ -2677,10 +2677,10 @@
         <v>172</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>50</v>
       </c>
@@ -2694,10 +2694,10 @@
         <v>169</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>51</v>
       </c>
@@ -2711,10 +2711,10 @@
         <v>26</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>52</v>
       </c>
@@ -2728,10 +2728,10 @@
         <v>159</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
@@ -2745,10 +2745,10 @@
         <v>121</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>54</v>
       </c>
@@ -2762,10 +2762,10 @@
         <v>113</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>55</v>
       </c>
@@ -2779,10 +2779,10 @@
         <v>153</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>56</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>57</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>123</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="10" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="10" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>59</v>
       </c>
@@ -2850,10 +2850,10 @@
         <v>58</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="10" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>60</v>
       </c>
@@ -2867,10 +2867,10 @@
         <v>271</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="10" customFormat="1" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="10" customFormat="1" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>61</v>
       </c>
@@ -2884,10 +2884,10 @@
         <v>271</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>62</v>
       </c>
@@ -2901,10 +2901,10 @@
         <v>174</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>63</v>
       </c>
@@ -2918,10 +2918,10 @@
         <v>171</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="10" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="10" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>64</v>
       </c>
@@ -2935,10 +2935,10 @@
         <v>173</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="10" customFormat="1" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="10" customFormat="1" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="19" t="s">
         <v>67</v>
       </c>
@@ -2952,10 +2952,10 @@
         <v>273</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="11" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>68</v>
       </c>
@@ -2969,10 +2969,10 @@
         <v>79</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="11" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>69</v>
       </c>
@@ -2986,10 +2986,10 @@
         <v>81</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="11" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="11" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>70</v>
       </c>
@@ -3003,10 +3003,10 @@
         <v>82</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="11" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>124</v>
       </c>
@@ -3020,10 +3020,10 @@
         <v>83</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="11" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="11" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>125</v>
       </c>
@@ -3037,10 +3037,10 @@
         <v>84</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="11" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="11" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>126</v>
       </c>
@@ -3054,10 +3054,10 @@
         <v>85</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="11" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="11" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>127</v>
       </c>
@@ -3071,10 +3071,10 @@
         <v>86</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="11" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>128</v>
       </c>
@@ -3088,10 +3088,10 @@
         <v>87</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="11" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>129</v>
       </c>
@@ -3105,10 +3105,10 @@
         <v>88</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="11" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="11" customFormat="1" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>130</v>
       </c>
@@ -3122,10 +3122,10 @@
         <v>89</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="11" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>131</v>
       </c>
@@ -3139,10 +3139,10 @@
         <v>90</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="11" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>132</v>
       </c>
@@ -3156,10 +3156,10 @@
         <v>91</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="11" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>133</v>
       </c>
@@ -3173,10 +3173,10 @@
         <v>92</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="11" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>134</v>
       </c>
@@ -3190,10 +3190,10 @@
         <v>93</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="11" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="11" customFormat="1" ht="79.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="19" t="s">
         <v>135</v>
       </c>
@@ -3207,10 +3207,10 @@
         <v>94</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="11" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="11" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>136</v>
       </c>
@@ -3224,10 +3224,10 @@
         <v>95</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="11" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="11" customFormat="1" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>137</v>
       </c>
@@ -3241,10 +3241,10 @@
         <v>96</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="11" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="11" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>138</v>
       </c>
@@ -3258,10 +3258,10 @@
         <v>98</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="11" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="11" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>139</v>
       </c>
@@ -3275,10 +3275,10 @@
         <v>99</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="11" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="11" customFormat="1" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>140</v>
       </c>
@@ -3292,10 +3292,10 @@
         <v>100</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" s="11" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="11" customFormat="1" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>141</v>
       </c>
@@ -3309,10 +3309,10 @@
         <v>101</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="11" customFormat="1" ht="128.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="11" customFormat="1" ht="132.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="19" t="s">
         <v>142</v>
       </c>
@@ -3326,10 +3326,10 @@
         <v>101</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="11" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="11" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>143</v>
       </c>
@@ -3343,10 +3343,10 @@
         <v>102</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="11" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>144</v>
       </c>
@@ -3360,10 +3360,10 @@
         <v>103</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="11" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="11" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>145</v>
       </c>
@@ -3377,10 +3377,10 @@
         <v>104</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="11" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>146</v>
       </c>
@@ -3394,10 +3394,10 @@
         <v>105</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" s="11" customFormat="1" ht="230.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="11" customFormat="1" ht="238.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="19" t="s">
         <v>147</v>
       </c>
@@ -3411,11 +3411,11 @@
         <v>208</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F77" s="12"/>
     </row>
-    <row r="78" spans="1:6" s="11" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" s="11" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>148</v>
       </c>
@@ -3429,11 +3429,11 @@
         <v>198</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F78" s="17"/>
     </row>
-    <row r="79" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>149</v>
       </c>
@@ -3451,7 +3451,7 @@
       </c>
       <c r="F79" s="11"/>
     </row>
-    <row r="80" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>150</v>
       </c>
@@ -3469,9 +3469,9 @@
       </c>
       <c r="F80" s="11"/>
     </row>
-    <row r="81" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>196</v>
@@ -3483,11 +3483,11 @@
         <v>72</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F81" s="17"/>
     </row>
-    <row r="82" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>151</v>
       </c>
@@ -3501,11 +3501,11 @@
         <v>73</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F82" s="17"/>
     </row>
-    <row r="83" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>152</v>
       </c>
@@ -3519,13 +3519,13 @@
         <v>73</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F83" s="17"/>
     </row>
-    <row r="84" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" ht="132" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>324</v>
@@ -3537,13 +3537,13 @@
         <v>74</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F84" s="11"/>
     </row>
-    <row r="85" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>203</v>
@@ -3555,13 +3555,13 @@
         <v>75</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F85" s="17"/>
     </row>
-    <row r="86" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>326</v>
@@ -3573,13 +3573,13 @@
         <v>76</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F86" s="11"/>
     </row>
-    <row r="87" spans="1:6" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>327</v>
@@ -3591,13 +3591,13 @@
         <v>77</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F87" s="11"/>
     </row>
-    <row r="88" spans="1:6" ht="90" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="93" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="19" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B88" s="20" t="s">
         <v>206</v>
@@ -3609,660 +3609,660 @@
         <v>78</v>
       </c>
       <c r="E88" s="22" t="s">
-        <v>351</v>
+        <v>414</v>
       </c>
       <c r="F88" s="18"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="C89" s="3"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
     </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
     </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
     </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
     </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
     </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
     </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
     </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" s="3"/>
       <c r="C193" s="3"/>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
     </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
     </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
     </row>
-    <row r="197" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
     </row>
-    <row r="198" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
     </row>
-    <row r="199" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
     </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
     </row>
-    <row r="201" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" s="3"/>
       <c r="C201" s="3"/>
     </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
     </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
     </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" s="3"/>
       <c r="C204" s="3"/>
     </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" s="3"/>
       <c r="C205" s="3"/>
     </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" s="3"/>
       <c r="C206" s="3"/>
     </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" s="3"/>
       <c r="C207" s="3"/>
     </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" s="3"/>
       <c r="C208" s="3"/>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" s="3"/>
       <c r="C209" s="3"/>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" s="3"/>
       <c r="C210" s="3"/>
     </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" s="3"/>
       <c r="C211" s="3"/>
     </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" s="3"/>
       <c r="C212" s="3"/>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" s="3"/>
       <c r="C213" s="3"/>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214" s="3"/>
       <c r="C214" s="3"/>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" s="3"/>
       <c r="C216" s="3"/>
     </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217" s="3"/>
       <c r="C217" s="3"/>
     </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" s="3"/>
       <c r="C218" s="3"/>
     </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" s="3"/>
       <c r="C219" s="3"/>
     </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
     </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" s="3"/>
       <c r="C221" s="3"/>
     </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" s="3"/>
       <c r="C222" s="3"/>
     </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
     </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" s="3"/>
       <c r="C224" s="3"/>
     </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225" s="3"/>
       <c r="C225" s="3"/>
     </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" s="3"/>
       <c r="C226" s="3"/>
     </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227" s="3"/>
       <c r="C227" s="3"/>
     </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228" s="3"/>
       <c r="C228" s="3"/>
     </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B229" s="3"/>
       <c r="C229" s="3"/>
     </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230" s="3"/>
       <c r="C230" s="3"/>
     </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231" s="3"/>
       <c r="C231" s="3"/>
     </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" s="3"/>
       <c r="C232" s="3"/>
     </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233" s="3"/>
       <c r="C233" s="3"/>
     </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B234" s="3"/>
       <c r="C234" s="3"/>
     </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B235" s="3"/>
       <c r="C235" s="3"/>
     </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B236" s="3"/>
       <c r="C236" s="3"/>
     </row>
-    <row r="237" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237" s="3"/>
       <c r="C237" s="3"/>
     </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238" s="3"/>
       <c r="C238" s="3"/>
     </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239" s="3"/>
       <c r="C239" s="3"/>
     </row>
-    <row r="240" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240" s="3"/>
       <c r="C240" s="3"/>
     </row>
-    <row r="241" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B241" s="3"/>
       <c r="C241" s="3"/>
     </row>
-    <row r="242" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B242" s="3"/>
       <c r="C242" s="3"/>
     </row>
-    <row r="243" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B243" s="3"/>
       <c r="C243" s="3"/>
     </row>
-    <row r="244" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B244" s="3"/>
       <c r="C244" s="3"/>
     </row>
-    <row r="245" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B245" s="3"/>
       <c r="C245" s="3"/>
     </row>
-    <row r="246" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B246" s="3"/>
       <c r="C246" s="3"/>
     </row>
-    <row r="247" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B247" s="3"/>
       <c r="C247" s="3"/>
     </row>
-    <row r="248" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B248" s="3"/>
       <c r="C248" s="3"/>
     </row>
-    <row r="249" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B249" s="3"/>
       <c r="C249" s="3"/>
     </row>
-    <row r="250" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B250" s="3"/>
       <c r="C250" s="3"/>
     </row>
-    <row r="251" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B251" s="3"/>
       <c r="C251" s="3"/>
     </row>
@@ -4284,6 +4284,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001DCD7BFB557E6E44A03D6903B90EA0A1" ma:contentTypeVersion="8" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="8436b4aaecc266f17e8e1c67f43e1083">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="afb956f7-b9fa-4db6-bd82-4239102aa811" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c05da2808cd4d9fa1eda7067bbba57fd" ns2:_="">
     <xsd:import namespace="afb956f7-b9fa-4db6-bd82-4239102aa811"/>
@@ -4455,12 +4461,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8CEECAF-EC76-4A1E-864B-AE8E1E6DABB1}">
   <ds:schemaRefs>
@@ -4470,6 +4470,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53A7212C-0BE6-40B0-8F0B-B781FEA2F273}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63E8A33E-6924-4B7B-B169-56068398ECDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4485,13 +4494,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53A7212C-0BE6-40B0-8F0B-B781FEA2F273}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>